<commit_message>
Makin' updates and changes
</commit_message>
<xml_diff>
--- a/public/data.xlsx
+++ b/public/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandon/Documents/web projects/college-counselor/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B60D69C8-B1B8-5743-A2D6-8F06F46B876F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20ACEB10-9A8B-1948-BDFC-9EDB8574D8E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{5E36B021-2387-A346-B1F0-D91A32F74C8B}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="16860" xr2:uid="{5E36B021-2387-A346-B1F0-D91A32F74C8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>University</t>
   </si>
@@ -90,19 +90,49 @@
   </si>
   <si>
     <t>Average Tuition</t>
+  </si>
+  <si>
+    <t>Bowling Green</t>
+  </si>
+  <si>
+    <t>Ohio</t>
+  </si>
+  <si>
+    <t>bgsu.edu</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Has Hospital</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -125,11 +155,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EF27CAD-D033-2549-AE6B-8142BDEAF702}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -457,7 +488,7 @@
     <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -473,8 +504,11 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -490,8 +524,11 @@
       <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -507,8 +544,11 @@
       <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="F3" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -524,8 +564,11 @@
       <c r="E4" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="F4" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -541,8 +584,11 @@
       <c r="E5" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="F5" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -557,6 +603,29 @@
       </c>
       <c r="E6" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1">
+        <v>185</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -566,6 +635,7 @@
     <hyperlink ref="E4" r:id="rId3" display="https://web.mit.edu/" xr:uid="{F3A558C9-01F7-BA4A-82E8-A0B35AEE7C2F}"/>
     <hyperlink ref="E3" r:id="rId4" display="https://www.harvard.edu/" xr:uid="{6C21CE37-3EE1-F141-9460-8DDFC627700B}"/>
     <hyperlink ref="E2" r:id="rId5" display="https://www.stanford.edu/" xr:uid="{4442D8CA-04B3-484E-AD06-81312D6DD8E2}"/>
+    <hyperlink ref="E7" r:id="rId6" display="https://www.cam.ac.uk/" xr:uid="{881BF329-137B-0747-A107-61393F556DD9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>